<commit_message>
kravspec och iteration v16
</commit_message>
<xml_diff>
--- a/Dokumentation/Iteration v15/Iteration 0.xlsx
+++ b/Dokumentation/Iteration v15/Iteration 0.xlsx
@@ -481,8 +481,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -642,7 +642,7 @@
         <v>16</v>
       </c>
       <c r="D13" s="3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E13" s="3">
         <v>10</v>
@@ -654,7 +654,9 @@
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
       <c r="E14" s="3">
         <v>0</v>
       </c>
@@ -716,12 +718,14 @@
         <v>26</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="D22" s="3">
         <v>3</v>
       </c>
-      <c r="E22" s="3"/>
+      <c r="E22" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
@@ -753,7 +757,9 @@
       <c r="D24" s="8">
         <v>3</v>
       </c>
-      <c r="E24" s="8"/>
+      <c r="E24" s="8">
+        <v>3</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -763,12 +769,14 @@
         <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>31</v>
+        <v>9</v>
       </c>
       <c r="D25" s="3">
         <v>6</v>
       </c>
-      <c r="E25" s="3"/>
+      <c r="E25" s="3">
+        <v>9</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
@@ -776,9 +784,11 @@
       <c r="C26" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>13</v>
+      </c>
       <c r="E26" s="3">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -787,7 +797,9 @@
       <c r="C27" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="3"/>
+      <c r="D27" s="3">
+        <v>8</v>
+      </c>
       <c r="E27" s="3">
         <v>10</v>
       </c>

</xml_diff>